<commit_message>
iterasi 3 with legend
</commit_message>
<xml_diff>
--- a/ProDS2/Prediction/iterasi3.xlsx
+++ b/ProDS2/Prediction/iterasi3.xlsx
@@ -1245,7 +1245,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>agriculture</t>
+          <t>land_without_scrub</t>
         </is>
       </c>
     </row>
@@ -1545,7 +1545,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>land_without_scrub</t>
         </is>
       </c>
     </row>
@@ -1797,7 +1797,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>land_without_scrub</t>
+          <t>river</t>
         </is>
       </c>
     </row>
@@ -2817,7 +2817,7 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>grassland</t>
+          <t>river</t>
         </is>
       </c>
     </row>
@@ -3345,7 +3345,7 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>crop</t>
+          <t>agriculture</t>
         </is>
       </c>
     </row>
@@ -4725,7 +4725,7 @@
       </c>
       <c r="B358" t="inlineStr">
         <is>
-          <t>land_without_scrub</t>
+          <t>agriculture</t>
         </is>
       </c>
     </row>
@@ -5109,7 +5109,7 @@
       </c>
       <c r="B390" t="inlineStr">
         <is>
-          <t>land_without_scrub</t>
+          <t>road_n_railway</t>
         </is>
       </c>
     </row>
@@ -5937,7 +5937,7 @@
       </c>
       <c r="B459" t="inlineStr">
         <is>
-          <t>agriculture</t>
+          <t>crop</t>
         </is>
       </c>
     </row>
@@ -6645,7 +6645,7 @@
       </c>
       <c r="B518" t="inlineStr">
         <is>
-          <t>agriculture</t>
+          <t>forest</t>
         </is>
       </c>
     </row>
@@ -6765,7 +6765,7 @@
       </c>
       <c r="B528" t="inlineStr">
         <is>
-          <t>forest</t>
+          <t>agriculture</t>
         </is>
       </c>
     </row>

</xml_diff>